<commit_message>
Final code and charts
</commit_message>
<xml_diff>
--- a/Top10.xlsx
+++ b/Top10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasmine\Documents\NSS\Projects\app-trader-fantastic-five\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE95D72A-CBB7-46FA-AC19-D73AF5A64D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7CA676-A026-4502-855A-75670CD57FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29025" yWindow="510" windowWidth="26010" windowHeight="15090" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Top10_ls" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -704,7 +704,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -752,30 +752,12 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -804,7 +786,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Top10.xlsx]Top10_ls_chart!PivotTable1</c:name>
+    <c:name>[Top10_v1.xlsx]Top10_ls_chart!PivotTable1</c:name>
     <c:fmtId val="2"/>
   </c:pivotSource>
   <c:chart>
@@ -1387,7 +1369,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent6">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
@@ -1410,8 +1392,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.12908177493438319"/>
-                  <c:y val="9.2720180810731953E-2"/>
+                  <c:x val="-0.13602608267716534"/>
+                  <c:y val="4.6423884514435694E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -1432,8 +1414,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.13689208770778652"/>
-                  <c:y val="-9.6175269757946921E-2"/>
+                  <c:x val="0.16467000218722661"/>
+                  <c:y val="-1.7471566054243305E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -1508,10 +1490,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11 years</c:v>
+                  <c:v>10 years</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10 years</c:v>
+                  <c:v>11 years</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1523,10 +1505,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1647,7 +1629,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Top10.xlsx]Top10_gr_chart!PivotTable3</c:name>
+    <c:name>[Top10_v1.xlsx]Top10_gr_chart!PivotTable3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2104,7 +2086,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Top10.xlsx]Top10_s_chart!PivotTable4</c:name>
+    <c:name>[Top10_v1.xlsx]Top10_s_chart!PivotTable4</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -9590,15 +9572,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>609599</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9663,12 +9645,11 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1200" b="1">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
             </a:rPr>
             <a:t>Total Lifespan:</a:t>
           </a:r>
@@ -9676,14 +9657,13 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US" sz="1200" b="1">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>103 years</a:t>
+            <a:t>106 years</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -11007,10 +10987,10 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of lifespan_years" fld="7" baseField="0" baseItem="0" numFmtId="173"/>
+    <dataField name="Sum of lifespan_years" fld="7" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -11219,7 +11199,7 @@
     <dataField name="Sum of total_revenue" fld="10" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="7">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -12076,8 +12056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12108,10 +12088,10 @@
         <v>10.8</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" s="5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -12122,10 +12102,10 @@
         <v>10.7</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="5">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -13117,7 +13097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A3:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>

</xml_diff>